<commit_message>
algunos cambios del articulo review
</commit_message>
<xml_diff>
--- a/Repositorio bibliografico.xlsx
+++ b/Repositorio bibliografico.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8d99fb567ae715c0/Escritorio/TRABALHOS EM JUPYTER/ARQUIVOS PHYTON/TRABALHO PROVA 3/Projecto em github/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="11" documentId="11_E5EA4401CE3BC786219EE382889A1D115891517F" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{21273200-0D55-478C-8E23-48238F35C909}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16950" windowHeight="6855"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Nome</t>
   </si>
@@ -83,13 +84,23 @@
     <t>DUD database</t>
   </si>
   <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>A mechanism-based 3D-QSAR approach for classification and prediction of acetylcholinesterase inhibitory potency of organophosphate and carbamate analogs</t>
+  </si>
+  <si>
+    <t>Development of dual inhibitors against Alzheimer’s disease using
+fragment-based QSAR and molecular docking</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Niu, B., Zhao, M., Su, Q., Zhang, M., Lv, W., Chen, Q., ... &amp; Zhang, Y. (2017). 2D-SAR and 3D-QSAR analyses for acetylcholinesterase inhibitors. </t>
     </r>
     <r>
       <rPr>
         <i/>
-        <sz val="11"/>
+        <sz val="10"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -99,7 +110,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
+        <sz val="10"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -110,7 +121,7 @@
     <r>
       <rPr>
         <i/>
-        <sz val="11"/>
+        <sz val="10"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -120,7 +131,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
+        <sz val="10"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -130,17 +141,14 @@
     </r>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>A mechanism-based 3D-QSAR approach for classification and prediction of acetylcholinesterase inhibitory potency of organophosphate and carbamate analogs</t>
+    <t>Goyal, M.; Dhanjal, J.K.; Goyal, S.; Tyagi, C.; Hamid, R.; Grover,A. Development of dual inhibitors against Alzheimer’s disease using fragment-based QSAR and molecular docking. BioMed Res. Int., 2014, 2014, 979606. [http://dx.doi.org/10.1155/2014/979606] [PMID: 25019089]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,8 +186,15 @@
       <family val="2"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -187,11 +202,25 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="10"/>
       <color theme="9" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -395,7 +424,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -406,18 +435,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -427,19 +447,29 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Encabezado 4" xfId="1" builtinId="19"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Título 4" xfId="1" builtinId="19"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -716,53 +746,53 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="F10" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" customWidth="1"/>
-    <col min="2" max="2" width="2.85546875" customWidth="1"/>
-    <col min="3" max="3" width="43.28515625" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="2.88671875" customWidth="1"/>
+    <col min="3" max="3" width="43.33203125" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
-    <col min="5" max="5" width="125.5703125" customWidth="1"/>
-    <col min="8" max="8" width="18.7109375" customWidth="1"/>
-    <col min="9" max="9" width="43" customWidth="1"/>
+    <col min="5" max="5" width="125.5546875" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" customWidth="1"/>
+    <col min="9" max="9" width="43" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="12" t="s">
+    <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="B3" s="8">
+    <row r="3" spans="2:9" ht="75.599999999999994" x14ac:dyDescent="0.3">
+      <c r="B3" s="5">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -774,25 +804,25 @@
       <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="9">
+      <c r="I3" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="6">
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" s="2">
         <v>2016</v>
@@ -801,10 +831,10 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="4"/>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="9">
+      <c r="I4" s="13"/>
+    </row>
+    <row r="5" spans="2:9" ht="15" x14ac:dyDescent="0.3">
+      <c r="B5" s="6">
         <v>3</v>
       </c>
       <c r="C5" s="2"/>
@@ -813,10 +843,10 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
-      <c r="I5" s="4"/>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="9">
+      <c r="I5" s="13"/>
+    </row>
+    <row r="6" spans="2:9" ht="15" x14ac:dyDescent="0.3">
+      <c r="B6" s="6">
         <v>4</v>
       </c>
       <c r="C6" s="2"/>
@@ -825,10 +855,10 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
-      <c r="I6" s="4"/>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="9">
+      <c r="I6" s="13"/>
+    </row>
+    <row r="7" spans="2:9" ht="15" x14ac:dyDescent="0.3">
+      <c r="B7" s="6">
         <v>5</v>
       </c>
       <c r="C7" s="2"/>
@@ -837,10 +867,10 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-      <c r="I7" s="4"/>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="8">
+      <c r="I7" s="13"/>
+    </row>
+    <row r="8" spans="2:9" ht="15" x14ac:dyDescent="0.3">
+      <c r="B8" s="5">
         <v>6</v>
       </c>
       <c r="C8" s="2"/>
@@ -849,10 +879,10 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
-      <c r="I8" s="4"/>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="9">
+      <c r="I8" s="13"/>
+    </row>
+    <row r="9" spans="2:9" ht="15" x14ac:dyDescent="0.3">
+      <c r="B9" s="6">
         <v>7</v>
       </c>
       <c r="C9" s="2"/>
@@ -861,10 +891,10 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
-      <c r="I9" s="4"/>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="9">
+      <c r="I9" s="13"/>
+    </row>
+    <row r="10" spans="2:9" ht="15" x14ac:dyDescent="0.3">
+      <c r="B10" s="6">
         <v>8</v>
       </c>
       <c r="C10" s="2"/>
@@ -873,10 +903,10 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
-      <c r="I10" s="4"/>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="9">
+      <c r="I10" s="13"/>
+    </row>
+    <row r="11" spans="2:9" ht="15" x14ac:dyDescent="0.3">
+      <c r="B11" s="6">
         <v>9</v>
       </c>
       <c r="C11" s="2"/>
@@ -885,10 +915,10 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
-      <c r="I11" s="4"/>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="9">
+      <c r="I11" s="13"/>
+    </row>
+    <row r="12" spans="2:9" ht="15" x14ac:dyDescent="0.3">
+      <c r="B12" s="6">
         <v>10</v>
       </c>
       <c r="C12" s="2"/>
@@ -897,10 +927,10 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
-      <c r="I12" s="4"/>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="8">
+      <c r="I12" s="13"/>
+    </row>
+    <row r="13" spans="2:9" ht="15" x14ac:dyDescent="0.3">
+      <c r="B13" s="5">
         <v>11</v>
       </c>
       <c r="C13" s="2"/>
@@ -909,10 +939,10 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
-      <c r="I13" s="4"/>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="9">
+      <c r="I13" s="13"/>
+    </row>
+    <row r="14" spans="2:9" ht="15" x14ac:dyDescent="0.3">
+      <c r="B14" s="6">
         <v>12</v>
       </c>
       <c r="C14" s="2"/>
@@ -921,10 +951,10 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
-      <c r="I14" s="4"/>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="9">
+      <c r="I14" s="13"/>
+    </row>
+    <row r="15" spans="2:9" ht="15" x14ac:dyDescent="0.3">
+      <c r="B15" s="6">
         <v>13</v>
       </c>
       <c r="C15" s="2"/>
@@ -933,10 +963,10 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
-      <c r="I15" s="4"/>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="9">
+      <c r="I15" s="13"/>
+    </row>
+    <row r="16" spans="2:9" ht="15" x14ac:dyDescent="0.3">
+      <c r="B16" s="6">
         <v>14</v>
       </c>
       <c r="C16" s="2"/>
@@ -945,10 +975,10 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
-      <c r="I16" s="4"/>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="9">
+      <c r="I16" s="13"/>
+    </row>
+    <row r="17" spans="2:9" ht="15" x14ac:dyDescent="0.3">
+      <c r="B17" s="6">
         <v>15</v>
       </c>
       <c r="C17" s="2"/>
@@ -957,10 +987,10 @@
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
-      <c r="I17" s="4"/>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="8">
+      <c r="I17" s="13"/>
+    </row>
+    <row r="18" spans="2:9" ht="15" x14ac:dyDescent="0.3">
+      <c r="B18" s="5">
         <v>16</v>
       </c>
       <c r="C18" s="2"/>
@@ -969,10 +999,10 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
-      <c r="I18" s="4"/>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="9">
+      <c r="I18" s="13"/>
+    </row>
+    <row r="19" spans="2:9" ht="15" x14ac:dyDescent="0.3">
+      <c r="B19" s="6">
         <v>17</v>
       </c>
       <c r="C19" s="2"/>
@@ -981,10 +1011,10 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
-      <c r="I19" s="4"/>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="9">
+      <c r="I19" s="13"/>
+    </row>
+    <row r="20" spans="2:9" ht="15" x14ac:dyDescent="0.3">
+      <c r="B20" s="6">
         <v>18</v>
       </c>
       <c r="C20" s="2"/>
@@ -993,10 +1023,10 @@
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
-      <c r="I20" s="4"/>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="9">
+      <c r="I20" s="13"/>
+    </row>
+    <row r="21" spans="2:9" ht="15" x14ac:dyDescent="0.3">
+      <c r="B21" s="6">
         <v>19</v>
       </c>
       <c r="C21" s="2"/>
@@ -1005,22 +1035,28 @@
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
-      <c r="I21" s="4"/>
-    </row>
-    <row r="22" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="10">
+      <c r="I21" s="13"/>
+    </row>
+    <row r="22" spans="2:9" ht="93" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="7">
         <v>20</v>
       </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
+      <c r="C22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="3">
+        <v>2014</v>
+      </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
-      <c r="I22" s="5"/>
+      <c r="I22" s="14" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
cambios no repositorio bibliografico e adição de novos artigos ao estado da arte
</commit_message>
<xml_diff>
--- a/Repositorio bibliografico.xlsx
+++ b/Repositorio bibliografico.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8d99fb567ae715c0/Escritorio/TRABALHOS EM JUPYTER/ARQUIVOS PHYTON/TRABALHO PROVA 3/Projecto em github/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="11_E5EA4401CE3BC786219EE382889A1D115891517F" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{21273200-0D55-478C-8E23-48238F35C909}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="11_E5EA4401CE3BC786219EE382889A1D115891517F" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B36E149A-C139-49CF-8B02-34F7EB803562}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-10164" yWindow="3468" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Nome</t>
   </si>
@@ -88,10 +88,6 @@
   </si>
   <si>
     <t>A mechanism-based 3D-QSAR approach for classification and prediction of acetylcholinesterase inhibitory potency of organophosphate and carbamate analogs</t>
-  </si>
-  <si>
-    <t>Development of dual inhibitors against Alzheimer’s disease using
-fragment-based QSAR and molecular docking</t>
   </si>
   <si>
     <r>
@@ -141,14 +137,79 @@
     </r>
   </si>
   <si>
-    <t>Goyal, M.; Dhanjal, J.K.; Goyal, S.; Tyagi, C.; Hamid, R.; Grover,A. Development of dual inhibitors against Alzheimer’s disease using fragment-based QSAR and molecular docking. BioMed Res. Int., 2014, 2014, 979606. [http://dx.doi.org/10.1155/2014/979606] [PMID: 25019089]</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Luan, F.; Cordeiro, M.N.; Alonso, N.; García-Mera, X.; Caamaño, O.; Romero-Duran, F.J.; Yañez, M.;  González-Díaz, H. TOPSMODE .model of multiplexing neuroprotective effects of drugs and experimental-theoretic study of new 1,3-rasagiline derivatives potentially useful in neurodegenerative diseases. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Bioorg. Med. Chem</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>., 2013, 21(7), 1870-1879. [http://dx.doi.org/10.1016/j.bmc.2013.01. 035] [PMID: 23415089]</t>
+    </r>
+  </si>
+  <si>
+    <t>TOPSMODE
+model of multiplexing neuroprotective effects of drugs and experimental- Theoretic study of new 1,3-rasagiline derivatives potentially useful in neurodegenerative diseases.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neste estudo foi usado o metodo multiplexing QSAR (mx-QSAR) para ensaios multiplos de molecuals bioativas da basede dados CHEMBL, eles apresentam uma Exatidão de 90%, sensitividade de 98% e seletividade de 80%  para o metodo LDA usado </t>
+  </si>
+  <si>
+    <t>LDA</t>
+  </si>
+  <si>
+    <t>CHEMBL</t>
+  </si>
+  <si>
+    <t>MODESLAB-metodo TOPS-MODE</t>
+  </si>
+  <si>
+    <t>Bautista-Aguilera, O.M.; Esteban, G.; Bolea, I.; Nikolic, K.; Agbaba,
+D.; Moraleda, I.; Iriepa, I.; Samadi, A.; Soriano, E.; Unzeta,
+M.; Marco-Contelles, J. Design, synthesis, pharmacological evaluation,
+QSAR analysis, molecular modeling and ADMET of novel
+donepezil-indolyl hybrids as multipotent cholinesterase/monoamine
+oxidase inhibitors for the potential treatment of Alzheimer’s disease.
+Eur. J. Med. Chem., 2014, 75, 82-95. [http://dx.doi.org/10.
+1016/j.ejmech.2013.12.028] [PMID: 24530494]</t>
+  </si>
+  <si>
+    <t>Design, synthesis, pharmacological evaluation, QSAR analysis, molecular modeling and ADMET of novel donepezil-indolyl hybrids as multipotent cholinesterase/monoamine oxidase inhibitors for the potential treatment of Alzheimer’s disease</t>
+  </si>
+  <si>
+    <t>PLS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Foram aplicados estudos famacoforicos e 3D-QSAR para desenhar uma serie de novos derivados da donezepila que podem inhibir tanto a AChE como a BChE, aí mostrou-se que tem inhibição no CAS e no PAS das enzimas usando o metodo do PLS.                                                                                                                                                                                  A seleção das variaveis foi feita usando PCA para o maping das estruturas e PLS para fazer a regreção junto com as variaveis descritoras para a valiar os modelos usou-se leave-one-out cross-validation Q2), correlation coefficient (R2 Observed vs. Predicted), Root Main Squared Error of Estimation (RMSEE), and external validation (Root Main Squared Error of Prediction (RMSEP)) </t>
+  </si>
+  <si>
+    <t>sintesis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -222,6 +283,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -463,7 +531,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -749,8 +817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F10" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -761,7 +829,7 @@
     <col min="4" max="4" width="9" customWidth="1"/>
     <col min="5" max="5" width="125.5546875" customWidth="1"/>
     <col min="8" max="8" width="18.6640625" customWidth="1"/>
-    <col min="9" max="9" width="43" style="10" customWidth="1"/>
+    <col min="9" max="9" width="66.21875" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -814,7 +882,7 @@
         <v>9</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1025,34 +1093,54 @@
       <c r="H20" s="2"/>
       <c r="I20" s="13"/>
     </row>
-    <row r="21" spans="2:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9" ht="112.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="6">
         <v>19</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
+      <c r="C21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="2">
+        <v>2014</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="H21" s="2"/>
-      <c r="I21" s="13"/>
-    </row>
-    <row r="22" spans="2:9" ht="93" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I21" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" ht="90.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="7">
         <v>20</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D22" s="3">
-        <v>2014</v>
-      </c>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
+        <v>2013</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="I22" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mais um artigo e modificação do repositorio bilbiografico
</commit_message>
<xml_diff>
--- a/Repositorio bibliografico.xlsx
+++ b/Repositorio bibliografico.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8d99fb567ae715c0/Escritorio/TRABALHOS EM JUPYTER/ARQUIVOS PHYTON/TRABALHO PROVA 3/Projecto em github/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="11_E5EA4401CE3BC786219EE382889A1D115891517F" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B36E149A-C139-49CF-8B02-34F7EB803562}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="11_E5EA4401CE3BC786219EE382889A1D115891517F" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{40E72270-6FAE-4EA8-96C3-A56863CFC0D1}"/>
   <bookViews>
-    <workbookView xWindow="-10164" yWindow="3468" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3084" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Nome</t>
   </si>
@@ -203,6 +203,33 @@
   </si>
   <si>
     <t>sintesis</t>
+  </si>
+  <si>
+    <t>Prado-Prado, F.; García-Mera, X.; Escobar, M.; Alonso, N.;
+Caamaño, O.; Yañez, M.; González-Díaz, H. 3D MI-DRAGON:
+new model for the reconstruction of US FDA drug- target network
+and theoretical-experimental studies of inhibitors of rasagiline derivatives
+for AChE. Curr. Top. Med. Chem., 2012, 12(16), 1843-
+1865. [http://dx.doi.org/10.2174/1568026611209061843] [PMID:
+23030618]</t>
+  </si>
+  <si>
+    <t>3D MI-DRAGON:new model for the reconstruction of US FDA drug- target network and theoretical-experimental studies of inhibitors of rasagiline derivatives for AChE</t>
+  </si>
+  <si>
+    <t>MLP(profile 37:37-24-1:1)</t>
+  </si>
+  <si>
+    <t>desenvolvimento de modelo 3D mt-QSAR para a predição de molecuals inhibidoras usando MI-DRAGON (MARCH-INSIDE e DRAGON) para calcular os descritores 3D para os compostos da DrugBank database. Foram usados algoritmos ANN para determinar o melhor modelo no linear. o modelo obteve 87,03% de exatidão, sensibilidade de 85,35% e seletividade de 87,48%</t>
+  </si>
+  <si>
+    <t>MI-DRAGON</t>
+  </si>
+  <si>
+    <t>3D-pharmacoporic</t>
+  </si>
+  <si>
+    <t>DrugBank</t>
   </si>
 </sst>
 </file>
@@ -305,7 +332,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -485,6 +512,15 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -492,7 +528,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -532,6 +568,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -818,7 +857,7 @@
   <dimension ref="B1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1081,17 +1120,31 @@
       <c r="H19" s="2"/>
       <c r="I19" s="13"/>
     </row>
-    <row r="20" spans="2:9" ht="15" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:9" ht="92.4" x14ac:dyDescent="0.3">
       <c r="B20" s="6">
         <v>18</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="13"/>
+      <c r="C20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="2">
+        <v>2012</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I20" s="13" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="21" spans="2:9" ht="112.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="6">
@@ -1112,7 +1165,9 @@
       <c r="G21" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H21" s="2"/>
+      <c r="H21" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="I21" s="13" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
por fin termine mi parte, casi que noo :(((
</commit_message>
<xml_diff>
--- a/Repositorio bibliografico.xlsx
+++ b/Repositorio bibliografico.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8d99fb567ae715c0/Escritorio/TRABALHOS EM JUPYTER/ARQUIVOS PHYTON/TRABALHO PROVA 3/Projecto em github/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="11_E5EA4401CE3BC786219EE382889A1D115891517F" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{831B2BBF-753C-43E4-84CA-AF674B4E966B}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="11_E5EA4401CE3BC786219EE382889A1D115891517F" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{2142B274-1177-43C7-A9DE-862C1E8CE160}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="105">
   <si>
     <t>Nome</t>
   </si>
@@ -228,89 +228,6 @@
 Probing the origins of human acetylcholinesterase inhibition via
 QSAR modeling and molecular docking. PeerJ, 2016, 4, e2322.
 [http://dx.doi.org/10.7717/peerj.2322] [PMID: 27602288]</t>
-  </si>
-  <si>
-    <t>The binding affinity was improved by the structural
-changes like: i) increase in molecular volume;
-ii) decrease in the energy of the LUMO; iii)
-insertion of a methylene group between the amide
-carbonyl and the aromatic ring; and iv) replacement of the amide oxygen by sulfur.   Derivatives of 2-
-amino-4,6-
-dimethylpyridine, aryl
-(alkyl) carboxamides,
-thiocarbamides and amidrazones.     2D-QSAR</t>
-  </si>
-  <si>
-    <t>Comparative 2DQSAR
-studies
-Three classes of
-AChEIs, for example,
-physostigmine analogs,
-1,2,3,4-
-tetrahydroacridines
-(tacrine analogs) and
-benzylamines
- i) Hydrophobicity plays a crucial role in both the
-physostigmine and the benzylamine-derived
-classes; ii) electronic effects are vital for the interactions
-shown by the variable portion of benzylamine
-derivatives; and iii) steric factors are also important</t>
-  </si>
-  <si>
-    <t>3D-QSAR models based on the flexible
-docking alignment
-using CoMFA and
-CoMSIA
-multi-target-directed
-AChEIs of tacrinenimodipine
-dihydropyridine
-AChE The results indicated that the IC50 can be improved
-by means of increasing the electronegativity and
-introducing small volume substituent at 3-position
-of the DHP (1,4-dihydropyridines) and hydrophobic
-like methoxy group was favorable to the 4-
-position of the benzene ring of DHP.</t>
-  </si>
-  <si>
-    <t>(GA)-MLR and
-(SA)-MLR
-Tacrine derivatives (a
-set of 80 structurally
-heterogeneous compounds
-composed of
-11H-indeno-[1,2-b]-
-quinolin-10-ylamine
-derivatives, thiopyranoquinolines,
-pyranoquinolines
-and benzonaphthyridines,
-tacrine-E2020 hybrids,
-bis-tacrine
-congeners, and
-tacrine-hurprine heterodimers)
-The best equation was obtained from SA MLR with
-greater explanatory and prediction capability. The
-results suggested the important roles of hydrophobic
-and electrostatic interactions on increasing the structure’s
-AChE activity.</t>
-  </si>
-  <si>
-    <t>3D-QSAR (CoMFA) study
-A series of 1-benzyl-
-4-[2-(N- benzoylamino)
-ethyl]
-piperidine derivatives
-and of Nbenzylpiperidine
-benzisoxazoles
-i) Substitutions with bulky and/or lipophilic groups at
-the benzisoxazole and benzoyl moieties are important
-for the activity;
-ii) The oxygen in isoxazole ring, if replaced with less
-electronegative atom like nitrogen or sulfur, is found
-to diminish the potency;
-iii) The basicity of the nitrogen atom in N-piperidine
-ring is important in contributing to the activity;
-iv) Occupying the ortho position of the benzoyl moiety
-with steric bulk negatively affects the activity.</t>
   </si>
   <si>
     <t>Tong, W.; Collantes, E.R.; Chen, Y.; Welsh, W.J. A comparative
@@ -505,6 +422,96 @@
   </si>
   <si>
     <t>bond fields. O modelo foi feito como a basede dados de 60 compostos derivados da tacrina, o composto com maior atividade inibidora foi usado como template e para as configurações dos metodos CoMFA e CoMSIA usou-se pra o primeiro valor predeterminado de  30 kcal·mol−1 para o campo esterico e eletrostatico no CoMFA  e os outros parametros deixaram-se predeterminados. Para o CoMSIA o calculo de 5 campos [steric, electrostatic, hydrophobic, hydrogen-bond (H-bond) donor and acceptor] foi avalidad usando a função Gaussiana e o fator de atenução foi de 0.3</t>
+  </si>
+  <si>
+    <t>metodo CoMFA e CoMSIA</t>
+  </si>
+  <si>
+    <t>Combined 3D-QSAR, molecular docking,  and molecular dynamics study of tacrine derivatives as potential acetylcholinesterase (AChE) inhibitors of  Alzheimer’s disease</t>
+  </si>
+  <si>
+    <t>Cholinesterase inhibition by derivatives of 2-amino-4,6-dimethylpyridine</t>
+  </si>
+  <si>
+    <t>Sintesis</t>
+  </si>
+  <si>
+    <t>automatic selection of
+the most significant variables, using the S-plus</t>
+  </si>
+  <si>
+    <t>linear regression</t>
+  </si>
+  <si>
+    <t>Neste trabalho foi feito um estudo2D- QSAR para a AChE e BChE onde foram testadas moleculas derivadas de  2- amino-4,6- dimethylpyridine, aryl (alkyl) carboxamides, thiocarbamides and amidrazones. a selelão dos descritores foi feita automaticamente pelo software S-plus deixando na equação aqueles com coeficientes de regressão significando  o nivel 5%.  A atividade foi calcualda experimentalmente aplicando o ensaio de Ellman modificado. segundo a analise feita  as carateristicas estruturais que melhoram a afinidade das moleculas pela diana alvo são : i) increase in molecular volume; ii) decrease in the energy of the LUMO; iii) insertion of a methylene group between the amide
+carbonyl and the aromatic ring; and iv) replacement of the amide oxygen by sulfur</t>
+  </si>
+  <si>
+    <t>program C-QSAR</t>
+  </si>
+  <si>
+    <t>A comparative QSAR
+analysis of acetylcholinesterase inhibitors currently studied for the
+treatment of Alzheimer’s disease</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Nesse artigo foi feito um estudo 2D-QSAR de tres classes de  inibidores AChE analogos de physostigmine, tacrine, benzylamines encontrando para cada um deles i) Hydrophobicity joga um papel importante na physostigmine e nos derivados da benzylamine; ii) electronic effects são de vital importancia pra as interações apresentadas dos derivados da benzylamine e  iii) steric factors é muito importante segundo a regressão feita pela metodologia.</t>
+  </si>
+  <si>
+    <t>3D-QSAR study of multi-target-directed AChE inhibitors based on autodocking</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CoMFA and CoMSIA methods</t>
+  </si>
+  <si>
+    <t>(Marco-Contelles et al.,
+2006a; Marco et al., 2001; Leon et al., 2008; Marco et al.,
+2004; Leon et al., 2005)</t>
+  </si>
+  <si>
+    <t>No estudo foi usado modelo 3D-QSAR baseado no linhamento deo docking usando CoMFA e CoMSIA para predizer a atividade biologica de tacrinenimodipine dihydropyridine derivates, o resultado identificou que  o IC50 pode melhorar com o incremento da electronegativity e a introdução de sustituentes de não voluminososna posição 3 das 1,4-dihydropyridines e grupos hidrofobicos como o metoxi e favoravel para a posição 4 no benzeno. a analise foi feita com 72 compostos divididos em 60 para o train e 12 para o teste.</t>
+  </si>
+  <si>
+    <t>A comparative molecular field analysis study of N-benzylpiperidines as  Acetylcholinesterase inhibitors</t>
+  </si>
+  <si>
+    <t>Quantitative structure-activity relationship (QSAR) of tacrine derivatives against  Acetylcholinesterase (AChE) activity using variable selection</t>
+  </si>
+  <si>
+    <t>11H-indeno-[1,2-b]-quinolin-10-ylamine derivatives,16
+thio-pyranoquinolines,17 pyranoquinolines and benzonaphthyridines,18–20 tacrine-E2020 hybrids,21 bis-tacrine
+congeners,22 and tacrine–hurprine heterodimers23 were
+taken from published results and used for the present
+QSAR study</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 133 descriptors was calculated for each compound in the data set by
+different kinds of software: 110 descriptors were calculated from PreADME on the Web,27 and 23 descriptors
+were obtained using the BioMedCAChe 6.10</t>
+  </si>
+  <si>
+    <t>(GA)-MLR and
+(SA)-MLR. software package SPSS 12.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+No estudo levado em consideração neste artigo foi feito um modelo QSAR usando metodologia Simulated annealing - MLR e Genetic algorithm-MLR com o passo de seleção de features. Comparando os resultados, para a construição do modelo foram utilizados dados de 80 estruturas de compostes heterogeneos, compostos por 11H-indeno-[1,2-b]- quinolin-10-ylamine derivatives, thiopyranoquinolines, pyranoquinolines and benzonaphthyridines, tacrine-E2020 hybrids, bis-tacrine congeners, and tacrine-hurprine heterodimers.  A melhor equação foi obtida pelo modelo SA-MLR com uma ampla explicação dos dados e uma boa capacidade de predição. o resultado permite definir propriedades significativas como hidrofobicidade e a interação eletrostatica que incrementa a atividade AChE, mas  a  hidrofilicidade e as carateristicas topologicas da molecula fazem com que a atividade diminua. a pre-seleção dos 32 descritores foi feita escolhendo aqueles como um coeficiente de correlção maior que 0,8. </t>
+  </si>
+  <si>
+    <t>Published in vitro biological data
+on a series of N-benzylpiperidine benzisoxazoles (NBPBs)7 and
+of 1-benzyl-4-[2-(N-benzoylamino)ethyl]piperidine derivatives
+(NBEPs)6 were used for this study</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CoMFA steric and electrostatic fields
+yielded </t>
+  </si>
+  <si>
+    <t>Este estudo  apresenta um modelo 3D-QSAR baseado na analise CoMFA  de derivados  1-benzyl-4-[2-(N- benzoylamino)ethyl piperidine e de  Nbenzylpiperidine benzisoxazoles. i) Substituções com grupos lipofilicos e voluminosos para os benzisoxazole e a porçao benzoyl são importantes para a atividade.
+ii)  O oxigenio no anel do isoxazole, se for trocado por um atomo com menor eletronegatividade como o nitrogenio ou o enxofre diminue a atividade biologica.
+iii) A basicidade do atomo do nitrogenio no anel da N-piperidine é importante na contribuição para atividade.
+iv) Ocupando na posição orto- da porção benzoyl com um grupo esterico volume esterico negativo afeta a atividade biologica.</t>
   </si>
 </sst>
 </file>
@@ -947,8 +954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -958,7 +965,7 @@
     <col min="3" max="3" width="43.33203125" style="9" customWidth="1"/>
     <col min="4" max="4" width="9" style="9" customWidth="1"/>
     <col min="5" max="5" width="125.5546875" style="9" customWidth="1"/>
-    <col min="6" max="6" width="11.5546875" style="14"/>
+    <col min="6" max="6" width="16.21875" style="14" customWidth="1"/>
     <col min="7" max="7" width="31.33203125" style="15" customWidth="1"/>
     <col min="8" max="8" width="37.6640625" style="15" customWidth="1"/>
     <col min="9" max="9" width="66.21875" style="15" customWidth="1"/>
@@ -1027,7 +1034,7 @@
         <v>9</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1196,25 +1203,25 @@
         <v>14</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D16" s="1">
         <v>2011</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="79.2" x14ac:dyDescent="0.3">
@@ -1223,25 +1230,25 @@
         <v>16</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D17" s="1">
         <v>2010</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="93.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1358,22 +1365,22 @@
         <v>21</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D22" s="6">
         <v>2009</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="I22" s="3" t="s">
         <v>38</v>
@@ -1385,22 +1392,22 @@
         <v>22</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D23" s="6">
         <v>2012</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F23" s="7" t="s">
         <v>22</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I23" s="3" t="s">
         <v>39</v>
@@ -1412,22 +1419,22 @@
         <v>23</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D24" s="6">
         <v>2006</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="I24" s="3" t="s">
         <v>40</v>
@@ -1439,22 +1446,22 @@
         <v>24</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D25" s="1">
         <v>2016</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="I25" s="3" t="s">
         <v>41</v>
@@ -1465,117 +1472,161 @@
       <c r="B26" s="13">
         <v>26</v>
       </c>
-      <c r="C26" s="1"/>
+      <c r="C26" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="D26" s="1">
         <v>2015</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="H26" s="3"/>
+        <v>80</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>82</v>
+      </c>
       <c r="I26" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="135" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="114.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6"/>
       <c r="B27" s="13">
         <v>28</v>
       </c>
-      <c r="C27" s="1"/>
+      <c r="C27" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="D27" s="1">
         <v>1997</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F27" s="2"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
+        <v>88</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>86</v>
+      </c>
       <c r="I27" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="210" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="132" x14ac:dyDescent="0.3">
       <c r="A28" s="6"/>
       <c r="B28" s="13">
         <v>29</v>
       </c>
-      <c r="C28" s="1"/>
+      <c r="C28" s="1" t="s">
+        <v>90</v>
+      </c>
       <c r="D28" s="1">
         <v>1997</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F28" s="2"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
+        <v>91</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="I28" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="195" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="84.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="6"/>
       <c r="B29" s="13">
         <v>30</v>
       </c>
-      <c r="C29" s="1"/>
+      <c r="C29" s="1" t="s">
+        <v>92</v>
+      </c>
       <c r="D29" s="1">
         <v>2012</v>
       </c>
       <c r="E29" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="I29" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F29" s="2"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="300" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:9" ht="156.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="6"/>
       <c r="B30" s="13">
         <v>31</v>
       </c>
-      <c r="C30" s="1"/>
+      <c r="C30" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="D30" s="1">
         <v>2007</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F30" s="2"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
+        <v>101</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="I30" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="255" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="120" x14ac:dyDescent="0.3">
       <c r="A31" s="6"/>
       <c r="B31" s="13">
         <v>32</v>
       </c>
-      <c r="C31" s="1"/>
+      <c r="C31" s="1" t="s">
+        <v>96</v>
+      </c>
       <c r="D31" s="1">
         <v>1996</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F31" s="2"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
+        <v>104</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="I31" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mi parte del repositorio segun archivo RAR
</commit_message>
<xml_diff>
--- a/Repositorio bibliografico.xlsx
+++ b/Repositorio bibliografico.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8d99fb567ae715c0/Escritorio/TRABALHOS EM JUPYTER/ARQUIVOS PHYTON/TRABALHO PROVA 3/Projecto em github/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Desktop\Trabalho Article\Model_Prediction_AChE_BA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="11_E5EA4401CE3BC786219EE382889A1D115891517F" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{21273200-0D55-478C-8E23-48238F35C909}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12720"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$B$1:$I$1</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="53">
   <si>
     <t>Nome</t>
   </si>
@@ -94,6 +96,9 @@
 fragment-based QSAR and molecular docking</t>
   </si>
   <si>
+    <t>Goyal, M.; Dhanjal, J.K.; Goyal, S.; Tyagi, C.; Hamid, R.; Grover,A. Development of dual inhibitors against Alzheimer’s disease using fragment-based QSAR and molecular docking. BioMed Res. Int., 2014, 2014, 979606. [http://dx.doi.org/10.1155/2014/979606] [PMID: 25019089]</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Niu, B., Zhao, M., Su, Q., Zhang, M., Lv, W., Chen, Q., ... &amp; Zhang, Y. (2017). 2D-SAR and 3D-QSAR analyses for acetylcholinesterase inhibitors. </t>
     </r>
@@ -102,9 +107,8 @@
         <i/>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>Molecular diversity</t>
     </r>
@@ -112,9 +116,8 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">, </t>
     </r>
@@ -123,9 +126,8 @@
         <i/>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>21</t>
     </r>
@@ -133,21 +135,252 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>(2), 413-426.</t>
     </r>
   </si>
   <si>
-    <t>Goyal, M.; Dhanjal, J.K.; Goyal, S.; Tyagi, C.; Hamid, R.; Grover,A. Development of dual inhibitors against Alzheimer’s disease using fragment-based QSAR and molecular docking. BioMed Res. Int., 2014, 2014, 979606. [http://dx.doi.org/10.1155/2014/979606] [PMID: 25019089]</t>
+    <r>
+      <t xml:space="preserve">Desenvolvimento de uma estrutura de previsão tridimensional para Ortofosfatos, carbamatos e seus análogos, as estruturas inibitórias de um composto que pode formar a ligação covalente foram identificadas através da análise das conformações em </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>docking</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> do composto e seus metabólitos. Potências inibitórias das estruturas selecionadas foram então previstas usando uma relação estrutura ativa quantitativa tridimensional previamente desenvolvida. </t>
+    </r>
+  </si>
+  <si>
+    <t>MOAtox</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Lee, S., &amp; Barron, M. G. (2016). A mechanism-based 3D-QSAR approach for classification and prediction of acetylcholinesterase inhibitory potency of organophosphate and carbamate analogs. Journal of computer-aided molecular design, 30(4), 347-363.</t>
+  </si>
+  <si>
+    <t>A QSAR study for the prediction of inhibitory activity of Coumarin derivatives for the treatment of Alzheimer’s Disease</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ghanei-Nasab, S., Hadizadeh, F., Foroumadi, A., &amp; Marjani, A. (2020). A QSAR Study for the Prediction of Inhibitory Activity of Coumarin Derivatives for the Treatment of Alzheimer’s Disease. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Arabian Journal for Science and Engineering</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, 1-9.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">MLR, PLS, RF, ANN, SVM </t>
+  </si>
+  <si>
+    <t>18/Dragon</t>
+  </si>
+  <si>
+    <t>Libsvm</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Aqui apresentam um estudo QSAR para prever a atividade inibitória (IC50) de derivados de cumarinas usando vários modelos de regressão estatística e aprendizado de máquina baseados em vários descritores moleculares de 94 compostos diferentes extraídos pelo  Dragon. Os modelos incluem MLR, PLS, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>random forest</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, redes neurais artificiais e SVM. Além disso, um algoritmo genético (GA) foi usado em combinação com MLR, PLS, SVM e ANN para encontrar um subconjunto menor dos descritores utilizados. Os resultados indicaram que o modelo GA-ANN atinge a melhor precisão de predição para IC50.</t>
+    </r>
+  </si>
+  <si>
+    <t>Zeng, H., &amp; Wu, X. (2016). Alzheimer's disease drug development based on Computer-Aided Drug Design. European journal of medicinal chemistry, 121, 851-863.</t>
+  </si>
+  <si>
+    <t>Alzheimer's disease drug development based on Computer-Aided Drug Design</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">LDA, SVM,ANN e </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>decision tree</t>
+    </r>
+  </si>
+  <si>
+    <t>ChEMBL</t>
+  </si>
+  <si>
+    <t>O presente estudo relata estudos QSAR em diversas classes químicas compreendendo 233 compostos. Aqui, modelos contínuos (regressão PLS e rede neural (NN)) e modelos QSAR categóricos (ANN e LDA) foram desenvolvidos para obter descritores pertinentes responsáveis pela variação da potência do inibidor de Gamma secretasa (um alvo de droga atraente para a doença de Alzheimer e câncer por causa de seu papel central no processamento da proteína precursora de amiloide e na família notch de proteínas) .</t>
+  </si>
+  <si>
+    <t>Evaluation of Amaryllidaceae alkaloids as inhibitors of human acetylcholinesterase by QSAR analysis and molecular docking</t>
+  </si>
+  <si>
+    <t>ChEMBL e NPASS</t>
+  </si>
+  <si>
+    <t>López, A. F. F., Martínez, O. M. M., &amp; Hernández, H. F. C. (2021). Evaluation of Amaryllidaceae alkaloids as inhibitors of human acetylcholinesterase by QSAR analysis and molecular docking. Journal of Molecular Structure, 1225, 129142.</t>
+  </si>
+  <si>
+    <t>1665/Volsurf e Dragon</t>
+  </si>
+  <si>
+    <t>1235/Adriana.code, MOE e Discovery</t>
+  </si>
+  <si>
+    <t>Binding DB</t>
+  </si>
+  <si>
+    <t>Fang, J., Yang, R., Gao, L., Zhou, D., Yang, S., Liu, A. L., &amp; Du, G. H. (2013). Predictions of BuChE inhibitors using support vector machine and naive Bayesian classification techniques in drug discovery. Journal of chemical information and modeling, 53(11), 3009-3020.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SVM e </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">naive Bayesian </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Nesta investigação, modelos SVM e modelos </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">naive Bayesian </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">foram construídos para discriminar os inibidores BuChE (BuChEIs) dos não inibidores. Cada molécula foi inicialmente representada em 1870 descritores estruturais. A análise de correlação e o método de seleção de variável stepwise foram aplicados para descobrir os descritores relacionados à atividade para modelos de previsão. Além disso, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>fingerprints</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> estruturais foram adicionados para melhorar a capacidade preditiva dos modelos, que foram medidos por validação cruzada, uma validação de conjunto de teste com 1001 compostos e uma validação de conjunto de teste externo com 317 produtos químicos diversos.</t>
+    </r>
+  </si>
+  <si>
+    <t>Predictions of BuChE Inhibitors Using Support Vector Machine and Naive Bayesian Classification Techniques in Drug Discovery</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Prediction of acetylcholinesterase inhibitors and characterization of correlative molecular descriptors by machine learning methods</t>
+  </si>
+  <si>
+    <t>SVM, k-NN, C4,5 DT</t>
+  </si>
+  <si>
+    <t>198/ Literatura</t>
+  </si>
+  <si>
+    <t>Literatura</t>
+  </si>
+  <si>
+    <t>Lv, W., &amp; Xue, Y. (2010). Prediction of acetylcholinesterase inhibitors and characterization of correlative molecular descriptors by machine learning methods. European journal of medicinal chemistry, 45(3), 1167-1172.</t>
+  </si>
+  <si>
+    <t>Neste trabalho, um método de seleção de características é usado para melhorar a precisão da predição e selecionar descritores moleculares responsáveis por distinguir IAChE e não IAChE. As precisões de previsão são 76,3% w88,0% para AChEIs e 74,3% w79,6% para não AChEIs com base nos três tipos de métodos de aprendizado de máquina. Este trabalho sugere que métodos de aprendizado de máquina como o SVM são facilitadores para prever o potencial de AChEIs de conjuntos desconhecidos de compostos e para exibir os descritores moleculares associados aos AChEIs.</t>
+  </si>
+  <si>
+    <t>Interpretation of toxicological activity of ionic liquids to acetylcholinesterase inhibition via in silico modelling</t>
+  </si>
+  <si>
+    <t>Predicting Inhibitors of Acetylcholinesterase by Regression and Classification Machine Learning Approaches with Combinations of Molecular Descriptors</t>
+  </si>
+  <si>
+    <t>Predicting acetyl cholinesterase enzyme inhibition potential of ionic liquids using machine learning approaches: An aid to green chemicals designing</t>
+  </si>
+  <si>
+    <t>MIA-QSAR based model for bioactivity prediction of flavonoid derivatives as acetylcholinesterase inhibitors</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -196,29 +429,27 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="9" tint="-0.499984740745262"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="12"/>
+      <color theme="9" tint="-0.499984740745262"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -237,7 +468,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -261,46 +492,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -424,52 +625,61 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Encabezado 4" xfId="1" builtinId="19"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Título 4" xfId="1" builtinId="19"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -746,316 +956,315 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:I22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F10" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" customWidth="1"/>
-    <col min="2" max="2" width="2.88671875" customWidth="1"/>
-    <col min="3" max="3" width="43.33203125" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" customWidth="1"/>
+    <col min="2" max="2" width="2.85546875" customWidth="1"/>
+    <col min="3" max="3" width="43.28515625" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
-    <col min="5" max="5" width="125.5546875" customWidth="1"/>
-    <col min="8" max="8" width="18.6640625" customWidth="1"/>
-    <col min="9" max="9" width="43" style="10" customWidth="1"/>
+    <col min="5" max="5" width="128.42578125" style="16" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" customWidth="1"/>
+    <col min="9" max="9" width="47.85546875" style="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="8" t="s">
+    <row r="1" spans="2:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I1" s="11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="75.599999999999994" x14ac:dyDescent="0.3">
-      <c r="B3" s="5">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
+    <row r="2" spans="2:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D2" s="1">
         <v>2016</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="12" t="s">
-        <v>15</v>
+      <c r="I2" s="10" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="6">
-        <v>2</v>
+    <row r="3" spans="2:9" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2016</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D4" s="2">
+        <v>2020</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="2">
+        <v>2015</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="2">
+        <v>2020</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="2">
         <v>2016</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="13"/>
-    </row>
-    <row r="5" spans="2:9" ht="15" x14ac:dyDescent="0.3">
-      <c r="B5" s="6">
-        <v>3</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="13"/>
-    </row>
-    <row r="6" spans="2:9" ht="15" x14ac:dyDescent="0.3">
-      <c r="B6" s="6">
-        <v>4</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="13"/>
-    </row>
-    <row r="7" spans="2:9" ht="15" x14ac:dyDescent="0.3">
-      <c r="B7" s="6">
-        <v>5</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-      <c r="I7" s="13"/>
+      <c r="I7" s="8"/>
     </row>
-    <row r="8" spans="2:9" ht="15" x14ac:dyDescent="0.3">
-      <c r="B8" s="5">
-        <v>6</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+    <row r="8" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="2">
+        <v>2018</v>
+      </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
-      <c r="I8" s="13"/>
+      <c r="I8" s="8"/>
     </row>
-    <row r="9" spans="2:9" ht="15" x14ac:dyDescent="0.3">
-      <c r="B9" s="6">
-        <v>7</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+    <row r="9" spans="2:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="2">
+        <v>2015</v>
+      </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
-      <c r="I9" s="13"/>
+      <c r="I9" s="8"/>
     </row>
-    <row r="10" spans="2:9" ht="15" x14ac:dyDescent="0.3">
-      <c r="B10" s="6">
-        <v>8</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+    <row r="10" spans="2:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="2">
+        <v>2009</v>
+      </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
-      <c r="I10" s="13"/>
+      <c r="I10" s="8"/>
     </row>
-    <row r="11" spans="2:9" ht="15" x14ac:dyDescent="0.3">
-      <c r="B11" s="6">
-        <v>9</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="13"/>
+    <row r="11" spans="2:9" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="2">
+        <v>2009</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="12" spans="2:9" ht="15" x14ac:dyDescent="0.3">
-      <c r="B12" s="6">
-        <v>10</v>
-      </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="13"/>
+    <row r="12" spans="2:9" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="2">
+        <v>2013</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="13" spans="2:9" ht="15" x14ac:dyDescent="0.3">
-      <c r="B13" s="5">
-        <v>11</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="13"/>
-    </row>
-    <row r="14" spans="2:9" ht="15" x14ac:dyDescent="0.3">
-      <c r="B14" s="6">
-        <v>12</v>
-      </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="13"/>
-    </row>
-    <row r="15" spans="2:9" ht="15" x14ac:dyDescent="0.3">
-      <c r="B15" s="6">
-        <v>13</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="13"/>
-    </row>
-    <row r="16" spans="2:9" ht="15" x14ac:dyDescent="0.3">
-      <c r="B16" s="6">
+    <row r="13" spans="2:9" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="13"/>
-    </row>
-    <row r="17" spans="2:9" ht="15" x14ac:dyDescent="0.3">
-      <c r="B17" s="6">
+      <c r="D13" s="3">
+        <v>2014</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="9" t="s">
         <v>15</v>
-      </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="13"/>
-    </row>
-    <row r="18" spans="2:9" ht="15" x14ac:dyDescent="0.3">
-      <c r="B18" s="5">
-        <v>16</v>
-      </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="13"/>
-    </row>
-    <row r="19" spans="2:9" ht="15" x14ac:dyDescent="0.3">
-      <c r="B19" s="6">
-        <v>17</v>
-      </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="13"/>
-    </row>
-    <row r="20" spans="2:9" ht="15" x14ac:dyDescent="0.3">
-      <c r="B20" s="6">
-        <v>18</v>
-      </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="13"/>
-    </row>
-    <row r="21" spans="2:9" ht="15" x14ac:dyDescent="0.3">
-      <c r="B21" s="6">
-        <v>19</v>
-      </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="13"/>
-    </row>
-    <row r="22" spans="2:9" ht="93" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="7">
-        <v>20</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D22" s="3">
-        <v>2014</v>
-      </c>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="14" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="B1:I1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualização final do repositorio
</commit_message>
<xml_diff>
--- a/Repositorio bibliografico.xlsx
+++ b/Repositorio bibliografico.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$B$2:$I$26</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="144">
   <si>
     <t>Nome</t>
   </si>
@@ -510,9 +513,6 @@
 iv) Ocupando na posição orto- da porção benzoyl com um grupo esterico volume esterico negativo afeta a atividade biologica.</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>A QSAR study for the prediction of inhibitory activity of Coumarin derivatives for the treatment of Alzheimer’s Disease</t>
   </si>
   <si>
@@ -755,12 +755,18 @@
   <si>
     <t>Para este estudo, os compostos no conjunto de teste foram cuidadosamente selecionados do conjunto original de estruturas e ambos conjuntos de treinamento e teste são estruturalmente diversos, cobrindo toda a gama de dados de atividade medida. Os conjuntos de treinamento e teste foram utilizados com estudos de regressão de SVR e PLS para permitir uma comparação quantitativa com modelos de regressão de PLS da literatura. Para análise de classificação, todo o conjunto de estruturas foi submetido à análise estatística para avaliar a qualidade do modelo. Usando strings SMILES dos artigos originais como entrada, para cada composto uma única conformação padrão de baixa energia foi gerada pelo software CORINA (Molecular Networks GmbH, Erlangen, German, http://www.mol-net.de).</t>
   </si>
+  <si>
+    <t>Dando uma olhada em as bases de dados: Web Of Sciencie, Scopus, Lens, SciencieDirect e Springer encontrou-se o que tem sido desenvolvido com a enzima AChE referente a os estudos QSAR por meio da implementação de bases de dados de diferentes moleculas com atividade biologica. Como proposta para o nosso trabalho, queremos desenvolver uma abordagem de diferentes tecnicas de aprendizado de maquina (SVM, MLPC, k-NN, LDA, QDA) para a criação de um modelo QSAR (2D e/ou 3D, fingerprints) para a predição da atividade biologica a partir das moleculas obtidas (em 3D ou nao) da base de dados BindingDBcontra AChE usando descritores AlvaDesc com filtragem (ou nao) segundo PCC maiores a 0,95.</t>
+  </si>
+  <si>
+    <t>S. Ajmani, S. Janardhan, V.N. Viswanadhan, Mol. Divers 17 (2013) 421e434</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -823,8 +829,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -837,8 +849,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -918,7 +936,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -936,10 +954,38 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -951,10 +997,25 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -970,21 +1031,6 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -997,9 +1043,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -1012,9 +1056,7 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -1025,7 +1067,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1066,9 +1108,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1078,37 +1117,43 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1392,11 +1437,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1405,7 +1450,7 @@
     <col min="2" max="2" width="4.42578125" style="7" customWidth="1"/>
     <col min="3" max="3" width="43.28515625" style="7" customWidth="1"/>
     <col min="4" max="4" width="9" style="7" customWidth="1"/>
-    <col min="5" max="5" width="125.5703125" style="15" customWidth="1"/>
+    <col min="5" max="5" width="125.5703125" style="14" customWidth="1"/>
     <col min="6" max="6" width="16.28515625" style="8" customWidth="1"/>
     <col min="7" max="7" width="31.28515625" style="9" customWidth="1"/>
     <col min="8" max="8" width="37.7109375" style="9" customWidth="1"/>
@@ -1413,682 +1458,702 @@
     <col min="10" max="16384" width="11.5703125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="23"/>
-      <c r="B1" s="25" t="s">
+    <row r="1" spans="1:9" ht="86.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="27" t="s">
+        <v>142</v>
+      </c>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="29"/>
+    </row>
+    <row r="2" spans="1:9" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="21"/>
+      <c r="B2" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F2" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="G2" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H2" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="28" t="s">
+      <c r="I2" s="26" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
-      <c r="B2" s="24">
+    <row r="3" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A3" s="21"/>
+      <c r="B3" s="22">
         <v>1</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C3" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" s="10">
+        <v>2020</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="21"/>
+      <c r="B4" s="15">
         <v>2</v>
       </c>
-      <c r="D2" s="10">
+      <c r="C4" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="21"/>
+      <c r="B5" s="22">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2018</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="21"/>
+      <c r="B6" s="15">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1">
         <v>2016</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I6" s="13" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="90" x14ac:dyDescent="0.2">
-      <c r="A3" s="23"/>
-      <c r="B3" s="16">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D3" s="1">
-        <v>2020</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="I3" s="14" t="s">
+    <row r="7" spans="1:9" ht="132" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="21"/>
+      <c r="B7" s="22">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2016</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="21"/>
+      <c r="B8" s="15">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
-      <c r="B4" s="16">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="D8" s="1">
+        <v>2015</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D4" s="1">
+      <c r="F8" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="21"/>
+      <c r="B9" s="22">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" s="1">
         <v>2015</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="I4" s="13" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="23"/>
-      <c r="B5" s="16">
-        <v>4</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D5" s="1">
-        <v>2020</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="I5" s="13" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="23"/>
-      <c r="B6" s="16">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D6" s="1">
-        <v>2018</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="I6" s="13" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
-      <c r="B7" s="16">
-        <v>6</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D7" s="1">
-        <v>2009</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="I7" s="13" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="23"/>
-      <c r="B8" s="16">
-        <v>7</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D8" s="1">
-        <v>2009</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="I8" s="13" t="s">
+      <c r="E9" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="21"/>
+      <c r="B10" s="15">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="1">
+        <v>2014</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="157.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="21"/>
+      <c r="B11" s="22">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="23"/>
-      <c r="B9" s="16">
-        <v>8</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="D11" s="1">
+        <v>2013</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D9" s="1">
+      <c r="F11" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12" s="21"/>
+      <c r="B12" s="15">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="1">
         <v>2013</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="I9" s="13" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="157.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="23"/>
-      <c r="B10" s="16">
-        <v>9</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="1">
-        <v>2011</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I10" s="13" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="23"/>
-      <c r="B11" s="16">
-        <v>10</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D11" s="1">
-        <v>2010</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="I11" s="13" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="93.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
-      <c r="B12" s="16">
+      <c r="E12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="93.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="21"/>
+      <c r="B13" s="22">
         <v>11</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="D12" s="1">
-        <v>2012</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I12" s="13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
-      <c r="B13" s="16">
-        <v>12</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="D13" s="1">
         <v>2012</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="21"/>
+      <c r="B14" s="15">
+        <v>12</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="1">
+        <v>2012</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G14" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="H14" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="I13" s="13" t="s">
+      <c r="I14" s="13" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="112.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="23"/>
-      <c r="B14" s="16">
+    <row r="15" spans="1:9" ht="112.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="21"/>
+      <c r="B15" s="22">
         <v>13</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="5">
+        <v>2012</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="94.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="21"/>
+      <c r="B16" s="15">
+        <v>14</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" s="1">
+        <v>2012</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="184.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="21"/>
+      <c r="B17" s="22">
+        <v>15</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="1">
+        <v>2011</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I17" s="13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="21"/>
+      <c r="B18" s="15">
+        <v>16</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="1">
+        <v>2010</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I18" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="146.44999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="21"/>
+      <c r="B19" s="22">
+        <v>17</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D19" s="1">
+        <v>2009</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="I19" s="13" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="127.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="21"/>
+      <c r="B20" s="15">
+        <v>18</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D20" s="1">
+        <v>2009</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="I20" s="13" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="180" x14ac:dyDescent="0.25">
+      <c r="A21" s="21"/>
+      <c r="B21" s="22">
+        <v>19</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="5">
+        <v>2009</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I21" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="159.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="21"/>
+      <c r="B22" s="15">
         <v>20</v>
       </c>
-      <c r="D14" s="1">
-        <v>2014</v>
-      </c>
-      <c r="E14" s="1" t="s">
+      <c r="C22" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D22" s="1">
+        <v>2007</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="I22" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A23" s="21"/>
+      <c r="B23" s="22">
+        <v>21</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D23" s="5">
+        <v>2006</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I23" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="21"/>
+      <c r="B24" s="15">
         <v>22</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="C24" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1997</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="I24" s="13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="156.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="21"/>
+      <c r="B25" s="22">
+        <v>23</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1997</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I25" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="21"/>
+      <c r="B26" s="15">
+        <v>24</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D26" s="17">
+        <v>1996</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="F26" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I14" s="13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="94.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="23"/>
-      <c r="B15" s="16">
-        <v>14</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="1">
-        <v>2013</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I15" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="184.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
-      <c r="B16" s="16">
-        <v>15</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" s="5">
-        <v>2009</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="I16" s="13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="23"/>
-      <c r="B17" s="16">
-        <v>16</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D17" s="5">
-        <v>2012</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="I17" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="146.44999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="23"/>
-      <c r="B18" s="16">
-        <v>17</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D18" s="5">
-        <v>2006</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="I18" s="13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="127.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
-      <c r="B19" s="16">
-        <v>18</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D19" s="1">
-        <v>2016</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="I19" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="23"/>
-      <c r="B20" s="16">
-        <v>19</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D20" s="1">
-        <v>2015</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="I20" s="13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="114.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="23"/>
-      <c r="B21" s="16">
-        <v>20</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D21" s="1">
-        <v>1997</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="I21" s="13" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="127.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="23"/>
-      <c r="B22" s="16">
-        <v>21</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D22" s="1">
-        <v>1997</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="I22" s="13" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="23"/>
-      <c r="B23" s="16">
-        <v>22</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D23" s="1">
-        <v>2012</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="I23" s="13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="156.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="23"/>
-      <c r="B24" s="16">
-        <v>23</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D24" s="1">
-        <v>2007</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="I24" s="13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="23"/>
-      <c r="B25" s="18">
-        <v>24</v>
-      </c>
-      <c r="C25" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="D25" s="19">
-        <v>1996</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="F25" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="G25" s="21" t="s">
+      <c r="G26" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="H25" s="21" t="s">
+      <c r="H26" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="I25" s="22" t="s">
+      <c r="I26" s="20" t="s">
         <v>41</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="B2:I26">
+    <sortState ref="B3:I26">
+      <sortCondition descending="1" ref="D2:D26"/>
+    </sortState>
+  </autoFilter>
+  <mergeCells count="1">
+    <mergeCell ref="B1:I1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>